<commit_message>
fix the bug: can't download pic from google
</commit_message>
<xml_diff>
--- a/excel_input/Hackathon 2025 Organizing Team Member Profile Submission.xlsx
+++ b/excel_input/Hackathon 2025 Organizing Team Member Profile Submission.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pytest\excel_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0FCEB03D-F7DE-46FE-A998-FE1621B600C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{48915BB9-BEB1-4266-8171-1A9F59A00354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15444" yWindow="4344" windowWidth="23724" windowHeight="13368" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15228" yWindow="2352" windowWidth="23724" windowHeight="13368" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="483">
   <si>
     <t>Id</t>
   </si>
@@ -271,9 +271,6 @@
     <t>Krishita</t>
   </si>
   <si>
-    <t>https://seneca.sharepoint.com/sites/2025HackathonPlanning/Shared%20Documents/Apps/Microsoft%20Forms/Hackathon%202025%20Organizing%20Team%20Member%20Profile%20Subm/Question/WhatsApp%20Image%202024-12-16%20at%2016.58.52_594aaaa_Krishita%20Nirmesh%20Vak.jpg</t>
-  </si>
-  <si>
     <t>https://www.linkedin.com/in/krishita-vakil-b37b53188/</t>
   </si>
   <si>
@@ -299,9 +296,6 @@
   </si>
   <si>
     <t>Rahul Amish Mamania</t>
-  </si>
-  <si>
-    <t>https://seneca.sharepoint.com/sites/2025HackathonPlanning/Shared%20Documents/Apps/Microsoft%20Forms/Hackathon%202025%20Organizing%20Team%20Member%20Profile%20Subm/Question/WhatsApp%20Image%202024-10-30%20at%2023.19.35_Rahul%20Amish%20Mamania.jpeg</t>
   </si>
   <si>
     <t>https://www.linkedin.com/in/rahul-mamania/</t>
@@ -1284,9 +1278,6 @@
     <t>2025-3-3 下午09:08:54</t>
   </si>
   <si>
-    <t>2025-3-3 下午09:15:45</t>
-  </si>
-  <si>
     <t>2025-3-3 下午09:16:25</t>
   </si>
   <si>
@@ -1312,9 +1303,6 @@
   </si>
   <si>
     <t>2025-3-4 下午06:46:26</t>
-  </si>
-  <si>
-    <t>2025-3-5 下午01:33:09</t>
   </si>
   <si>
     <t>2025-3-5 下午09:19:39</t>
@@ -1350,9 +1338,6 @@
     <t>aa8@myseneca.ca</t>
   </si>
   <si>
-    <t>cjbuenaventura@myseneca.ca</t>
-  </si>
-  <si>
     <t>vsavchyn@myseneca.ca</t>
   </si>
   <si>
@@ -1420,9 +1405,6 @@
     <t>Utpal Manishchandra Prajapati</t>
   </si>
   <si>
-    <t>Num</t>
-  </si>
-  <si>
     <t>Siddhi Patel</t>
   </si>
   <si>
@@ -1435,9 +1417,6 @@
     <t>https://drive.google.com/open?id=1omRCdXrgpM0zmuPKzd45X5cy3P99Jv2V</t>
   </si>
   <si>
-    <t>https://drive.google.com/open?id=1PQ7LaNzV-mbmWh0hLPhF2Y2MwVKcpuR9</t>
-  </si>
-  <si>
     <t>https://drive.google.com/open?id=1kRjZhsDtRHjqIoDSNc_EDsbudLdzg50s</t>
   </si>
   <si>
@@ -1450,9 +1429,6 @@
     <t>https://drive.google.com/open?id=1y7P6kSnPO3nLp0wlXo9As6w1GtZixkYs</t>
   </si>
   <si>
-    <t>https://drive.google.com/open?id=1HA9k5zKKLL1Ko6LDw_0sPQyHwfKBwHVC</t>
-  </si>
-  <si>
     <t>https://drive.google.com/open?id=1wotF5RzvgbShFtBqVGbj-VM-2cJfnP9M</t>
   </si>
   <si>
@@ -1465,9 +1441,6 @@
     <t>https://drive.google.com/open?id=1rWpo-efL-DfqKQjOFeI5JUrI2nRyu-a_</t>
   </si>
   <si>
-    <t>https://drive.google.com/open?id=14kBdmcWhUM5qHieKgrQNHfgUGK-CPkb-</t>
-  </si>
-  <si>
     <t>https://drive.google.com/open?id=18i1lXKp99NvgcoSg_QF1r77sLpIt2CsT</t>
   </si>
   <si>
@@ -1507,9 +1480,6 @@
     <t>www.linkedin.com/in/utpal-prajapati-191a391a8</t>
   </si>
   <si>
-    <t>www.linkedin.com/in/num-praditsakul-67a629132</t>
-  </si>
-  <si>
     <t>https://www.linkedin.com/in/siddhipatel10/</t>
   </si>
   <si>
@@ -1519,9 +1489,6 @@
     <t>Software Development Team Lead</t>
   </si>
   <si>
-    <t>Senior Consultant</t>
-  </si>
-  <si>
     <t>Backend Tester: Tested backend API with Jest and Supertest. Sometimes tested front-end.</t>
   </si>
   <si>
@@ -1538,9 +1505,6 @@
   </si>
   <si>
     <t>student success officer</t>
-  </si>
-  <si>
-    <t>QA/QC Manager</t>
   </si>
   <si>
     <t>Data Analytics</t>
@@ -1559,6 +1523,26 @@
   </si>
   <si>
     <t>Fenil Mehta</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>cjbuenaventura@myseneca.ca</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cleo Buenaventura</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1HA9k5zKKLL1Ko6LDw_0sPQyHwfKBwHVC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1VYrkf61sKKEovtaPPXKQJoEft9UKxmM7</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1nBgDszp_I0qFXi6Z94V0JSIkWaZ972jv</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1685,8 +1669,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="OfficeForms.Table" displayName="OfficeForms.Table" ref="A1:K81" totalsRowShown="0">
-  <autoFilter ref="A1:K81" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="OfficeForms.Table" displayName="OfficeForms.Table" ref="A1:K79" totalsRowShown="0">
+  <autoFilter ref="A1:K79" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K66">
     <sortCondition ref="K1:K66"/>
   </sortState>
@@ -2087,10 +2071,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K81"/>
+  <dimension ref="A1:K79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="D88" sqref="D88"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A79" sqref="A79:XFD79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -2148,26 +2132,26 @@
         <v>45686.661909722199</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="H2" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="G2" s="4" t="s">
+      <c r="I2" s="5" t="s">
         <v>290</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>292</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="28.8" x14ac:dyDescent="0.25">
@@ -2181,26 +2165,26 @@
         <v>45680.598993055602</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="G3" s="4" t="s">
+      <c r="I3" s="5" t="s">
         <v>220</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>222</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -2214,28 +2198,28 @@
         <v>45683.844085648103</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="G4" s="4" t="s">
+      <c r="I4" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="K4" t="s">
         <v>248</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="K4" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="28.8" x14ac:dyDescent="0.25">
@@ -2249,26 +2233,26 @@
         <v>45686.812164351897</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>329</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="G5" s="4" t="s">
         <v>331</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="I5" s="5" t="s">
         <v>333</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>335</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -2282,26 +2266,26 @@
         <v>45685.709444444401</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="G6" s="4" t="s">
+      <c r="I6" s="5" t="s">
         <v>259</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>261</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -2315,26 +2299,26 @@
         <v>45686.6856134259</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="H7" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="G7" s="4" t="s">
+      <c r="I7" s="5" t="s">
         <v>296</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>298</v>
       </c>
       <c r="J7" s="2"/>
       <c r="K7" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.25">
@@ -2348,26 +2332,26 @@
         <v>45682.553495370397</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="G8" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="I8" s="5" t="s">
         <v>233</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>235</v>
       </c>
       <c r="J8" s="2"/>
       <c r="K8" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="43.2" x14ac:dyDescent="0.25">
@@ -2381,26 +2365,26 @@
         <v>45686.958634259303</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>343</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="H9" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>344</v>
-      </c>
-      <c r="G9" s="4" t="s">
+      <c r="I9" s="5" t="s">
         <v>345</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>347</v>
       </c>
       <c r="J9" s="2"/>
       <c r="K9" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="57.6" x14ac:dyDescent="0.25">
@@ -2414,26 +2398,26 @@
         <v>45687.001516203702</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>349</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="H10" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="G10" s="4" t="s">
+      <c r="I10" s="5" t="s">
         <v>351</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>353</v>
       </c>
       <c r="J10" s="2"/>
       <c r="K10" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="57.6" x14ac:dyDescent="0.25">
@@ -2447,26 +2431,26 @@
         <v>45691.847048611096</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="G11" s="4" t="s">
         <v>387</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="H11" s="4" t="s">
         <v>388</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>388</v>
-      </c>
-      <c r="G11" s="4" t="s">
+      <c r="I11" s="5" t="s">
         <v>389</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>390</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>391</v>
       </c>
       <c r="J11" s="2"/>
       <c r="K11" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="360" x14ac:dyDescent="0.25">
@@ -2480,28 +2464,28 @@
         <v>45675.022870370398</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G12" s="4" t="s">
+      <c r="I12" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="J12" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="K12" t="s">
         <v>149</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="K12" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="57.6" x14ac:dyDescent="0.25">
@@ -2515,26 +2499,26 @@
         <v>45682.619467592602</v>
       </c>
       <c r="D13" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="G13" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="H13" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="I13" s="5" t="s">
         <v>240</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>242</v>
       </c>
       <c r="J13" s="2"/>
       <c r="K13" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -2548,28 +2532,28 @@
         <v>45688.854733796303</v>
       </c>
       <c r="D14" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>367</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="G14" s="4" t="s">
         <v>368</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="H14" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="G14" s="4" t="s">
+      <c r="I14" s="5" t="s">
         <v>370</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="J14" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="I14" s="5" t="s">
-        <v>372</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>373</v>
-      </c>
       <c r="K14" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -2583,26 +2567,26 @@
         <v>45686.839953703697</v>
       </c>
       <c r="D15" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="G15" s="4" t="s">
         <v>337</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="H15" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="I15" s="5" t="s">
         <v>339</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>341</v>
       </c>
       <c r="J15" s="2"/>
       <c r="K15" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -2616,26 +2600,26 @@
         <v>45686.764386574097</v>
       </c>
       <c r="D16" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="G16" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="H16" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="G16" s="4" t="s">
+      <c r="I16" s="5" t="s">
         <v>326</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>328</v>
       </c>
       <c r="J16" s="2"/>
       <c r="K16" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="43.2" x14ac:dyDescent="0.25">
@@ -2649,26 +2633,26 @@
         <v>45688.7755092593</v>
       </c>
       <c r="D17" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>360</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="G17" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="H17" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="I17" s="5" t="s">
         <v>364</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>365</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>366</v>
       </c>
       <c r="J17" s="2"/>
       <c r="K17" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="57.6" x14ac:dyDescent="0.25">
@@ -2682,26 +2666,26 @@
         <v>45689.734270833302</v>
       </c>
       <c r="D18" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="G18" s="4" t="s">
         <v>374</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="H18" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="G18" s="4" t="s">
+      <c r="I18" s="5" t="s">
         <v>376</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>378</v>
       </c>
       <c r="J18" s="2"/>
       <c r="K18" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="129.6" x14ac:dyDescent="0.25">
@@ -2715,26 +2699,26 @@
         <v>45685.985578703701</v>
       </c>
       <c r="D19" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="G19" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="H19" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="I19" s="5" t="s">
         <v>284</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>286</v>
       </c>
       <c r="J19" s="2"/>
       <c r="K19" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -2748,26 +2732,26 @@
         <v>45686.719745370399</v>
       </c>
       <c r="D20" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="G20" s="4" t="s">
         <v>318</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="H20" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="G20" s="4" t="s">
+      <c r="I20" s="5" t="s">
         <v>320</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>322</v>
       </c>
       <c r="J20" s="2"/>
       <c r="K20" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="115.2" x14ac:dyDescent="0.25">
@@ -2781,26 +2765,26 @@
         <v>45692.681608796302</v>
       </c>
       <c r="D21" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>392</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="G21" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="H21" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="G21" s="4" t="s">
+      <c r="I21" s="5" t="s">
         <v>395</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>396</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>397</v>
       </c>
       <c r="J21" s="2"/>
       <c r="K21" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -2814,26 +2798,26 @@
         <v>45709.002928240698</v>
       </c>
       <c r="D22" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>397</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="G22" s="4" t="s">
         <v>399</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="H22" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="I22" s="5" t="s">
         <v>401</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="I22" s="5" t="s">
-        <v>403</v>
       </c>
       <c r="J22" s="2"/>
       <c r="K22" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="86.4" x14ac:dyDescent="0.25">
@@ -2847,28 +2831,28 @@
         <v>45675.769027777802</v>
       </c>
       <c r="D23" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="G23" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="H23" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="F23" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="G23" s="4" t="s">
+      <c r="I23" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="H23" s="4" t="s">
+      <c r="J23" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="I23" s="5" t="s">
+      <c r="K23" t="s">
         <v>174</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="K23" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -2882,26 +2866,26 @@
         <v>45675.693761574097</v>
       </c>
       <c r="D24" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="G24" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="H24" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="F24" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="G24" s="4" t="s">
+      <c r="I24" s="5" t="s">
         <v>160</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="I24" s="5" t="s">
-        <v>162</v>
       </c>
       <c r="J24" s="2"/>
       <c r="K24" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="43.2" x14ac:dyDescent="0.25">
@@ -2915,26 +2899,26 @@
         <v>45675.401875000003</v>
       </c>
       <c r="D25" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="G25" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="H25" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="F25" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G25" s="4" t="s">
+      <c r="I25" s="5" t="s">
         <v>154</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>156</v>
       </c>
       <c r="J25" s="2"/>
       <c r="K25" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -2948,26 +2932,26 @@
         <v>45681.803356481498</v>
       </c>
       <c r="D26" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="G26" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="H26" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="F26" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="G26" s="4" t="s">
+      <c r="I26" s="5" t="s">
         <v>226</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="I26" s="5" t="s">
-        <v>228</v>
       </c>
       <c r="J26" s="2"/>
       <c r="K26" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="43.2" x14ac:dyDescent="0.25">
@@ -2981,26 +2965,26 @@
         <v>45685.871701388904</v>
       </c>
       <c r="D27" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="F27" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="E27" s="6" t="s">
+      <c r="G27" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="H27" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="G27" s="4" t="s">
+      <c r="I27" s="5" t="s">
         <v>266</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="I27" s="5" t="s">
-        <v>268</v>
       </c>
       <c r="J27" s="2"/>
       <c r="K27" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -3014,26 +2998,26 @@
         <v>45677.600173611099</v>
       </c>
       <c r="D28" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="F28" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="G28" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="H28" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="G28" s="4" t="s">
+      <c r="I28" s="5" t="s">
         <v>187</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>189</v>
       </c>
       <c r="J28" s="2"/>
       <c r="K28" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="72" x14ac:dyDescent="0.25">
@@ -3047,26 +3031,26 @@
         <v>45685.920983796299</v>
       </c>
       <c r="D29" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="G29" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="E29" s="6" t="s">
+      <c r="H29" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="F29" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="G29" s="4" t="s">
+      <c r="I29" s="5" t="s">
         <v>272</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="I29" s="5" t="s">
-        <v>274</v>
       </c>
       <c r="J29" s="2"/>
       <c r="K29" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="129.6" x14ac:dyDescent="0.25">
@@ -3080,26 +3064,26 @@
         <v>45686.704814814802</v>
       </c>
       <c r="D30" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="G30" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="E30" s="6" t="s">
+      <c r="H30" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="F30" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="G30" s="4" t="s">
+      <c r="I30" s="5" t="s">
         <v>315</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="I30" s="5" t="s">
-        <v>317</v>
       </c>
       <c r="J30" s="2"/>
       <c r="K30" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="115.2" x14ac:dyDescent="0.25">
@@ -3113,26 +3097,26 @@
         <v>45679.8380555556</v>
       </c>
       <c r="D31" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="G31" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="H31" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="F31" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="G31" s="4" t="s">
+      <c r="I31" s="5" t="s">
         <v>208</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="I31" s="5" t="s">
-        <v>210</v>
       </c>
       <c r="J31" s="2"/>
       <c r="K31" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="72" x14ac:dyDescent="0.25">
@@ -3146,26 +3130,26 @@
         <v>45684.941180555601</v>
       </c>
       <c r="D32" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="G32" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="H32" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="F32" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="G32" s="4" t="s">
+      <c r="I32" s="5" t="s">
         <v>253</v>
-      </c>
-      <c r="H32" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="I32" s="5" t="s">
-        <v>255</v>
       </c>
       <c r="J32" s="2"/>
       <c r="K32" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="72" x14ac:dyDescent="0.25">
@@ -3179,26 +3163,26 @@
         <v>45679.736539351899</v>
       </c>
       <c r="D33" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="F33" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="G33" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="H33" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="G33" s="4" t="s">
+      <c r="I33" s="5" t="s">
         <v>202</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="I33" s="5" t="s">
-        <v>204</v>
       </c>
       <c r="J33" s="2"/>
       <c r="K33" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="158.4" x14ac:dyDescent="0.25">
@@ -3212,26 +3196,26 @@
         <v>45675.751585648097</v>
       </c>
       <c r="D34" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G34" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="H34" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="F34" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="G34" s="4" t="s">
+      <c r="I34" s="5" t="s">
         <v>166</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="I34" s="5" t="s">
-        <v>168</v>
       </c>
       <c r="J34" s="2"/>
       <c r="K34" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="72" x14ac:dyDescent="0.25">
@@ -3245,26 +3229,26 @@
         <v>45679.839710648099</v>
       </c>
       <c r="D35" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="F35" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="E35" s="6" t="s">
+      <c r="G35" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="H35" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="G35" s="4" t="s">
+      <c r="I35" s="5" t="s">
         <v>215</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="I35" s="5" t="s">
-        <v>217</v>
       </c>
       <c r="J35" s="2"/>
       <c r="K35" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="86.4" x14ac:dyDescent="0.25">
@@ -3278,26 +3262,26 @@
         <v>45689.762974537</v>
       </c>
       <c r="D36" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="F36" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="E36" s="6" t="s">
+      <c r="G36" s="4" t="s">
         <v>381</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="H36" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="G36" s="4" t="s">
+      <c r="I36" s="5" t="s">
         <v>383</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="I36" s="5" t="s">
-        <v>385</v>
       </c>
       <c r="J36" s="2"/>
       <c r="K36" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="43.2" x14ac:dyDescent="0.25">
@@ -3311,26 +3295,26 @@
         <v>45676.635625000003</v>
       </c>
       <c r="D37" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="F37" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="G37" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="H37" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="G37" s="4" t="s">
+      <c r="I37" s="5" t="s">
         <v>180</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="I37" s="5" t="s">
-        <v>182</v>
       </c>
       <c r="J37" s="2"/>
       <c r="K37" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="86.4" x14ac:dyDescent="0.25">
@@ -3344,26 +3328,26 @@
         <v>45685.925451388903</v>
       </c>
       <c r="D38" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="G38" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="E38" s="6" t="s">
+      <c r="H38" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="F38" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="G38" s="4" t="s">
+      <c r="I38" s="5" t="s">
         <v>277</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="I38" s="5" t="s">
-        <v>279</v>
       </c>
       <c r="J38" s="2"/>
       <c r="K38" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="28.8" x14ac:dyDescent="0.25">
@@ -3377,26 +3361,26 @@
         <v>45687.533773148098</v>
       </c>
       <c r="D39" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="G39" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="E39" s="6" t="s">
+      <c r="H39" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="F39" s="2" t="s">
-        <v>356</v>
-      </c>
-      <c r="G39" s="4" t="s">
+      <c r="I39" s="5" t="s">
         <v>357</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="I39" s="5" t="s">
-        <v>359</v>
       </c>
       <c r="J39" s="2"/>
       <c r="K39" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="302.39999999999998" x14ac:dyDescent="0.25">
@@ -3410,28 +3394,28 @@
         <v>45678.003009259301</v>
       </c>
       <c r="D40" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F40" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="G40" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="H40" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="G40" s="4" t="s">
+      <c r="I40" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="H40" s="2" t="s">
+      <c r="J40" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="I40" s="5" t="s">
+      <c r="K40" t="s">
         <v>196</v>
-      </c>
-      <c r="J40" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="K40" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="57.6" x14ac:dyDescent="0.25">
@@ -3445,26 +3429,26 @@
         <v>45686.686006944401</v>
       </c>
       <c r="D41" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="G41" s="4" t="s">
         <v>300</v>
       </c>
-      <c r="E41" s="6" t="s">
+      <c r="H41" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="F41" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="G41" s="4" t="s">
+      <c r="I41" s="5" t="s">
         <v>302</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="I41" s="5" t="s">
-        <v>304</v>
       </c>
       <c r="J41" s="2"/>
       <c r="K41" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="72" x14ac:dyDescent="0.25">
@@ -3478,26 +3462,26 @@
         <v>45686.697708333297</v>
       </c>
       <c r="D42" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="F42" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="E42" s="6" t="s">
+      <c r="G42" s="4" t="s">
         <v>307</v>
       </c>
-      <c r="F42" s="2" t="s">
+      <c r="H42" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="G42" s="4" t="s">
+      <c r="I42" s="5" t="s">
         <v>309</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="I42" s="5" t="s">
-        <v>311</v>
       </c>
       <c r="J42" s="2"/>
       <c r="K42" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -3851,13 +3835,13 @@
         <v>75</v>
       </c>
       <c r="G54" s="4" t="s">
+        <v>482</v>
+      </c>
+      <c r="H54" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="H54" s="2" t="s">
+      <c r="I54" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="I54" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="J54" s="2"/>
     </row>
@@ -3872,22 +3856,22 @@
         <v>45664.804675925901</v>
       </c>
       <c r="D55" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E55" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E55" s="2" t="s">
+      <c r="F55" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G55" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="F55" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="G55" s="4" t="s">
+      <c r="H55" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H55" s="2" t="s">
+      <c r="I55" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="I55" s="2" t="s">
-        <v>83</v>
       </c>
       <c r="J55" s="2"/>
     </row>
@@ -3902,22 +3886,22 @@
         <v>45665.212673611102</v>
       </c>
       <c r="D56" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E56" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E56" s="2" t="s">
+      <c r="F56" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G56" s="4" t="s">
+        <v>481</v>
+      </c>
+      <c r="H56" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="F56" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="G56" s="4" t="s">
+      <c r="I56" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="H56" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="I56" s="2" t="s">
-        <v>88</v>
       </c>
       <c r="J56" s="2"/>
     </row>
@@ -3932,22 +3916,22 @@
         <v>45665.533773148098</v>
       </c>
       <c r="D57" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G57" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="E57" s="2" t="s">
+      <c r="H57" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F57" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="G57" s="4" t="s">
+      <c r="I57" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="H57" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I57" s="5" t="s">
-        <v>93</v>
       </c>
       <c r="J57" s="2"/>
     </row>
@@ -3962,22 +3946,22 @@
         <v>45665.657627314802</v>
       </c>
       <c r="D58" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F58" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E58" s="2" t="s">
+      <c r="G58" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="F58" s="2" t="s">
+      <c r="H58" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="G58" s="4" t="s">
+      <c r="I58" s="5" t="s">
         <v>97</v>
-      </c>
-      <c r="H58" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="I58" s="5" t="s">
-        <v>99</v>
       </c>
       <c r="J58" s="2"/>
     </row>
@@ -3992,25 +3976,25 @@
         <v>45665.724722222199</v>
       </c>
       <c r="D59" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F59" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E59" s="2" t="s">
+      <c r="G59" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="F59" s="2" t="s">
+      <c r="H59" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="G59" s="4" t="s">
+      <c r="I59" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="H59" s="2" t="s">
+      <c r="J59" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="I59" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="J59" s="2" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
@@ -4024,22 +4008,22 @@
         <v>45665.881087962996</v>
       </c>
       <c r="D60" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F60" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E60" s="2" t="s">
+      <c r="G60" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="F60" s="2" t="s">
+      <c r="H60" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="G60" s="4" t="s">
+      <c r="I60" s="5" t="s">
         <v>110</v>
-      </c>
-      <c r="H60" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="I60" s="5" t="s">
-        <v>112</v>
       </c>
       <c r="J60" s="2"/>
     </row>
@@ -4054,22 +4038,22 @@
         <v>45665.903078703697</v>
       </c>
       <c r="D61" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F61" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E61" s="2" t="s">
+      <c r="G61" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="F61" s="2" t="s">
+      <c r="H61" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="G61" s="4" t="s">
+      <c r="I61" s="5" t="s">
         <v>116</v>
-      </c>
-      <c r="H61" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="I61" s="5" t="s">
-        <v>118</v>
       </c>
       <c r="J61" s="2"/>
     </row>
@@ -4084,22 +4068,22 @@
         <v>45666.902361111097</v>
       </c>
       <c r="D62" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="G62" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="E62" s="2" t="s">
+      <c r="H62" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="F62" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="G62" s="4" t="s">
+      <c r="I62" s="5" t="s">
         <v>121</v>
-      </c>
-      <c r="H62" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="I62" s="5" t="s">
-        <v>123</v>
       </c>
       <c r="J62" s="2"/>
     </row>
@@ -4114,22 +4098,22 @@
         <v>45667.474525463003</v>
       </c>
       <c r="D63" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="G63" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="E63" s="2" t="s">
+      <c r="H63" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="F63" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="G63" s="4" t="s">
+      <c r="I63" s="5" t="s">
         <v>126</v>
-      </c>
-      <c r="H63" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="I63" s="5" t="s">
-        <v>128</v>
       </c>
       <c r="J63" s="2"/>
     </row>
@@ -4144,22 +4128,22 @@
         <v>45667.490335648203</v>
       </c>
       <c r="D64" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G64" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="E64" s="2" t="s">
+      <c r="H64" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="F64" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="G64" s="4" t="s">
+      <c r="I64" s="5" t="s">
         <v>131</v>
-      </c>
-      <c r="H64" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="I64" s="5" t="s">
-        <v>133</v>
       </c>
       <c r="J64" s="2"/>
     </row>
@@ -4174,22 +4158,22 @@
         <v>45668.655092592599</v>
       </c>
       <c r="D65" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="G65" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="E65" s="2" t="s">
+      <c r="H65" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="F65" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="G65" s="4" t="s">
+      <c r="I65" s="5" t="s">
         <v>136</v>
-      </c>
-      <c r="H65" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="I65" s="5" t="s">
-        <v>138</v>
       </c>
       <c r="J65" s="2"/>
     </row>
@@ -4204,386 +4188,338 @@
         <v>45670.655057870397</v>
       </c>
       <c r="D66" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F66" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="E66" s="2" t="s">
+      <c r="G66" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="F66" s="2" t="s">
+      <c r="H66" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="G66" s="4" t="s">
+      <c r="I66" s="5" t="s">
         <v>142</v>
-      </c>
-      <c r="H66" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="I66" s="5" t="s">
-        <v>144</v>
       </c>
       <c r="J66" s="2"/>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C67" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="D67" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="E67" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="F67" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="H67" s="3" t="s">
-        <v>461</v>
+        <v>452</v>
       </c>
       <c r="I67" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="J67" s="2"/>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C68" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D68" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E68" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="F68" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
       <c r="H68" s="3" t="s">
-        <v>462</v>
+        <v>453</v>
       </c>
       <c r="I68" s="5" t="s">
-        <v>475</v>
+        <v>465</v>
       </c>
       <c r="J68" s="2"/>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C69" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D69" t="s">
+        <v>424</v>
+      </c>
+      <c r="E69" t="s">
         <v>429</v>
       </c>
-      <c r="E69" t="s">
-        <v>434</v>
-      </c>
       <c r="F69" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="H69" s="3" t="s">
-        <v>463</v>
+        <v>454</v>
       </c>
       <c r="I69" s="5" t="s">
-        <v>476</v>
+        <v>466</v>
       </c>
       <c r="J69" s="2"/>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C70" t="s">
+        <v>404</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>478</v>
+      </c>
+      <c r="E70" t="s">
+        <v>479</v>
+      </c>
+      <c r="F70" t="s">
+        <v>430</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>443</v>
+      </c>
+      <c r="H70" s="3" t="s">
+        <v>455</v>
+      </c>
+      <c r="I70" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="J70" s="2"/>
+    </row>
+    <row r="71" spans="1:10" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
+        <v>405</v>
+      </c>
+      <c r="D71" t="s">
+        <v>417</v>
+      </c>
+      <c r="E71" t="s">
+        <v>431</v>
+      </c>
+      <c r="F71" t="s">
+        <v>431</v>
+      </c>
+      <c r="G71" s="3" t="s">
+        <v>444</v>
+      </c>
+      <c r="H71" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="I71" s="5" t="s">
+        <v>467</v>
+      </c>
+      <c r="J71" s="2"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
         <v>406</v>
       </c>
-      <c r="D70" t="s">
-        <v>324</v>
-      </c>
-      <c r="E70" t="s">
-        <v>325</v>
-      </c>
-      <c r="F70" t="s">
-        <v>325</v>
-      </c>
-      <c r="G70" s="3" t="s">
-        <v>449</v>
-      </c>
-      <c r="H70" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="I70" s="5" t="s">
-        <v>477</v>
-      </c>
-      <c r="J70" s="2"/>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C71" t="s">
-        <v>407</v>
-      </c>
-      <c r="D71" t="s">
-        <v>421</v>
-      </c>
-      <c r="E71" t="s">
-        <v>435</v>
-      </c>
-      <c r="F71" t="s">
-        <v>435</v>
-      </c>
-      <c r="G71" s="3" t="s">
-        <v>450</v>
-      </c>
-      <c r="H71" s="3" t="s">
-        <v>464</v>
-      </c>
-      <c r="I71" s="5" t="s">
-        <v>328</v>
-      </c>
-      <c r="J71" s="2"/>
-    </row>
-    <row r="72" spans="1:10" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="C72" t="s">
-        <v>408</v>
-      </c>
       <c r="D72" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="E72" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F72" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="H72" s="3" t="s">
-        <v>465</v>
+        <v>457</v>
       </c>
       <c r="I72" s="5" t="s">
-        <v>478</v>
+        <v>468</v>
       </c>
       <c r="J72" s="2"/>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C73" t="s">
+        <v>407</v>
+      </c>
+      <c r="D73" t="s">
+        <v>419</v>
+      </c>
+      <c r="E73" t="s">
+        <v>433</v>
+      </c>
+      <c r="F73" t="s">
+        <v>433</v>
+      </c>
+      <c r="G73" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="H73" s="3" t="s">
+        <v>458</v>
+      </c>
+      <c r="I73" s="5" t="s">
+        <v>474</v>
+      </c>
+      <c r="J73" s="2" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="C74" t="s">
+        <v>408</v>
+      </c>
+      <c r="D74" t="s">
+        <v>420</v>
+      </c>
+      <c r="E74" t="s">
+        <v>434</v>
+      </c>
+      <c r="F74" t="s">
+        <v>477</v>
+      </c>
+      <c r="G74" s="3" t="s">
+        <v>480</v>
+      </c>
+      <c r="H74" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="I74" s="5" t="s">
+        <v>476</v>
+      </c>
+      <c r="J74" s="2"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C75" t="s">
         <v>409</v>
       </c>
-      <c r="D73" t="s">
-        <v>423</v>
-      </c>
-      <c r="E73" t="s">
-        <v>437</v>
-      </c>
-      <c r="F73" t="s">
-        <v>437</v>
-      </c>
-      <c r="G73" s="3" t="s">
-        <v>452</v>
-      </c>
-      <c r="H73" s="3" t="s">
-        <v>466</v>
-      </c>
-      <c r="I73" s="5" t="s">
-        <v>479</v>
-      </c>
-      <c r="J73" s="2"/>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C74" t="s">
-        <v>410</v>
-      </c>
-      <c r="D74" t="s">
-        <v>424</v>
-      </c>
-      <c r="E74" t="s">
-        <v>438</v>
-      </c>
-      <c r="F74" t="s">
-        <v>438</v>
-      </c>
-      <c r="G74" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="H74" s="3" t="s">
-        <v>467</v>
-      </c>
-      <c r="I74" s="5" t="s">
-        <v>486</v>
-      </c>
-      <c r="J74" s="2" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" ht="43.2" x14ac:dyDescent="0.25">
-      <c r="C75" t="s">
-        <v>411</v>
-      </c>
       <c r="D75" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="E75" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="F75" t="s">
-        <v>489</v>
+        <v>435</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
       <c r="H75" s="3" t="s">
-        <v>468</v>
+        <v>460</v>
       </c>
       <c r="I75" s="5" t="s">
-        <v>488</v>
+        <v>469</v>
       </c>
       <c r="J75" s="2"/>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C76" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D76" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="E76" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="F76" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>455</v>
+        <v>448</v>
       </c>
       <c r="H76" s="3" t="s">
-        <v>469</v>
+        <v>461</v>
       </c>
       <c r="I76" s="5" t="s">
-        <v>480</v>
+        <v>470</v>
       </c>
       <c r="J76" s="2"/>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C77" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D77" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="E77" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="F77" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="H77" s="3" t="s">
-        <v>470</v>
+        <v>462</v>
       </c>
       <c r="I77" s="5" t="s">
-        <v>481</v>
+        <v>471</v>
       </c>
       <c r="J77" s="2"/>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C78" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D78" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="E78" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="F78" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="H78" s="3" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
       <c r="I78" s="5" t="s">
-        <v>482</v>
+        <v>472</v>
       </c>
       <c r="J78" s="2"/>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C79" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D79" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="E79" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="F79" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>458</v>
+        <v>451</v>
       </c>
       <c r="H79" s="3" t="s">
-        <v>472</v>
+        <v>464</v>
       </c>
       <c r="I79" s="5" t="s">
-        <v>483</v>
+        <v>473</v>
       </c>
       <c r="J79" s="2"/>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C80" t="s">
-        <v>416</v>
-      </c>
-      <c r="D80" t="s">
-        <v>11</v>
-      </c>
-      <c r="E80" t="s">
-        <v>444</v>
-      </c>
-      <c r="F80" t="s">
-        <v>444</v>
-      </c>
-      <c r="G80" s="3" t="s">
-        <v>459</v>
-      </c>
-      <c r="H80" s="3" t="s">
-        <v>473</v>
-      </c>
-      <c r="I80" s="5" t="s">
-        <v>484</v>
-      </c>
-      <c r="J80" s="2"/>
-    </row>
-    <row r="81" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C81" t="s">
-        <v>417</v>
-      </c>
-      <c r="D81" t="s">
-        <v>431</v>
-      </c>
-      <c r="E81" t="s">
-        <v>445</v>
-      </c>
-      <c r="F81" t="s">
-        <v>445</v>
-      </c>
-      <c r="G81" s="3" t="s">
-        <v>460</v>
-      </c>
-      <c r="H81" s="3" t="s">
-        <v>474</v>
-      </c>
-      <c r="I81" s="5" t="s">
-        <v>485</v>
-      </c>
-      <c r="J81" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -4640,42 +4576,39 @@
     <hyperlink ref="H23" r:id="rId50" xr:uid="{9E2E8F65-A9B3-49F2-8F64-D29DBE4E02FC}"/>
     <hyperlink ref="H28" r:id="rId51" xr:uid="{6172FC36-6AFE-47AE-954D-8F45FE05E6AA}"/>
     <hyperlink ref="H32" r:id="rId52" xr:uid="{A82EEFC3-966F-41E4-8B80-1D5962557BB7}"/>
-    <hyperlink ref="D81" r:id="rId53" xr:uid="{0CEFF791-E95D-4ABA-A862-DF8D25286141}"/>
+    <hyperlink ref="D79" r:id="rId53" xr:uid="{0CEFF791-E95D-4ABA-A862-DF8D25286141}"/>
     <hyperlink ref="G67" r:id="rId54" xr:uid="{0A8DB93B-F23F-41D3-B86D-4E7800374184}"/>
     <hyperlink ref="G68" r:id="rId55" xr:uid="{A4702360-8338-4834-BBB3-4DA3784826ED}"/>
     <hyperlink ref="G69" r:id="rId56" xr:uid="{4EFD3C91-6A9B-47B1-8FE5-28B1BF9F1758}"/>
-    <hyperlink ref="G70" r:id="rId57" xr:uid="{3377676B-ABF0-4B52-98D1-674FFCFF5E65}"/>
-    <hyperlink ref="G71" r:id="rId58" xr:uid="{0ADCBA34-E341-4D56-BA72-1CFCB176C002}"/>
-    <hyperlink ref="G72" r:id="rId59" xr:uid="{99EFED3C-1D54-4D1C-951E-2BB803D11455}"/>
-    <hyperlink ref="G73" r:id="rId60" xr:uid="{E1CF2291-F7F8-43BB-BAE3-6CA8E28E69DC}"/>
-    <hyperlink ref="G74" r:id="rId61" xr:uid="{61C89F6A-E0C7-481B-B046-9070DFEAA7B0}"/>
-    <hyperlink ref="G75" r:id="rId62" xr:uid="{EED23829-C10A-4AC4-A8C4-7E5E0BC04332}"/>
-    <hyperlink ref="G76" r:id="rId63" xr:uid="{9F47E65B-ADD3-4696-9F22-4616E13ACA8C}"/>
-    <hyperlink ref="G77" r:id="rId64" xr:uid="{003A8779-C298-46D9-99C9-B4E1BD48DE13}"/>
-    <hyperlink ref="G78" r:id="rId65" xr:uid="{C1801A5C-C80E-4A15-BA09-6ADCEA403351}"/>
-    <hyperlink ref="G79" r:id="rId66" xr:uid="{781A5559-115C-4236-B90B-6370F8DDE613}"/>
-    <hyperlink ref="G80" r:id="rId67" xr:uid="{A5CC7275-040F-47EC-97C7-EF5675DBA84C}"/>
-    <hyperlink ref="G81" r:id="rId68" xr:uid="{1F30A8EE-EABA-4782-B4C9-AF65846F2783}"/>
-    <hyperlink ref="H67" r:id="rId69" xr:uid="{53FA6DF3-8C37-48D4-8816-1E80C8D579E0}"/>
-    <hyperlink ref="H68" r:id="rId70" xr:uid="{9281E405-2B8F-4887-9335-CBDC6DA92955}"/>
-    <hyperlink ref="H69" r:id="rId71" xr:uid="{32E88D78-E9D5-4F1C-9310-49AD01D6A7F4}"/>
-    <hyperlink ref="H70" r:id="rId72" xr:uid="{7CA3B2D0-B930-43B4-8BE5-E88FBB1C7979}"/>
-    <hyperlink ref="H71" r:id="rId73" display="http://linkedin.com/in/cleo-buenaventura" xr:uid="{AD76BCF3-33C1-4BF3-A3C2-635342E614A9}"/>
-    <hyperlink ref="H72" r:id="rId74" xr:uid="{CADE8B5C-A2FF-48E1-8E62-A8B2727C383F}"/>
-    <hyperlink ref="H73" r:id="rId75" xr:uid="{99C2B4AC-06EC-445C-AD10-96989F1C25E0}"/>
-    <hyperlink ref="H74" r:id="rId76" xr:uid="{86078F22-8AF1-44CD-BEAC-01233F855721}"/>
-    <hyperlink ref="H75" r:id="rId77" display="http://www.linkedin.com/in/suhana-shrestha" xr:uid="{53C26434-110F-4AF6-8CD6-9A93C8475C92}"/>
-    <hyperlink ref="H76" r:id="rId78" xr:uid="{6F73D0A1-C18C-438B-AC1D-94521C25804F}"/>
-    <hyperlink ref="H77" r:id="rId79" display="http://www.linkedin.com/in/tomisin-ojaokomo" xr:uid="{88EDD760-8E2F-43EC-9B0D-2FAD141AA86E}"/>
-    <hyperlink ref="H78" r:id="rId80" xr:uid="{F51A016D-E482-4ABD-94F9-394B4880D096}"/>
-    <hyperlink ref="H79" r:id="rId81" display="http://www.linkedin.com/in/utpal-prajapati-191a391a8" xr:uid="{B173318C-C519-4672-A834-1FF1FFF1A8E0}"/>
-    <hyperlink ref="H80" r:id="rId82" display="http://www.linkedin.com/in/num-praditsakul-67a629132" xr:uid="{CB8C2458-2E38-49F6-8FB4-98E9EAEE0542}"/>
-    <hyperlink ref="H81" r:id="rId83" xr:uid="{6FE58E59-576D-40AD-821D-BAD2429E40BC}"/>
+    <hyperlink ref="G70" r:id="rId57" xr:uid="{0ADCBA34-E341-4D56-BA72-1CFCB176C002}"/>
+    <hyperlink ref="G71" r:id="rId58" xr:uid="{99EFED3C-1D54-4D1C-951E-2BB803D11455}"/>
+    <hyperlink ref="G72" r:id="rId59" xr:uid="{E1CF2291-F7F8-43BB-BAE3-6CA8E28E69DC}"/>
+    <hyperlink ref="G73" r:id="rId60" xr:uid="{61C89F6A-E0C7-481B-B046-9070DFEAA7B0}"/>
+    <hyperlink ref="G74" r:id="rId61" xr:uid="{EED23829-C10A-4AC4-A8C4-7E5E0BC04332}"/>
+    <hyperlink ref="G75" r:id="rId62" xr:uid="{9F47E65B-ADD3-4696-9F22-4616E13ACA8C}"/>
+    <hyperlink ref="G76" r:id="rId63" xr:uid="{003A8779-C298-46D9-99C9-B4E1BD48DE13}"/>
+    <hyperlink ref="G77" r:id="rId64" xr:uid="{C1801A5C-C80E-4A15-BA09-6ADCEA403351}"/>
+    <hyperlink ref="G78" r:id="rId65" xr:uid="{781A5559-115C-4236-B90B-6370F8DDE613}"/>
+    <hyperlink ref="G79" r:id="rId66" xr:uid="{1F30A8EE-EABA-4782-B4C9-AF65846F2783}"/>
+    <hyperlink ref="H67" r:id="rId67" xr:uid="{53FA6DF3-8C37-48D4-8816-1E80C8D579E0}"/>
+    <hyperlink ref="H68" r:id="rId68" xr:uid="{9281E405-2B8F-4887-9335-CBDC6DA92955}"/>
+    <hyperlink ref="H69" r:id="rId69" xr:uid="{32E88D78-E9D5-4F1C-9310-49AD01D6A7F4}"/>
+    <hyperlink ref="H70" r:id="rId70" display="http://linkedin.com/in/cleo-buenaventura" xr:uid="{AD76BCF3-33C1-4BF3-A3C2-635342E614A9}"/>
+    <hyperlink ref="H71" r:id="rId71" xr:uid="{CADE8B5C-A2FF-48E1-8E62-A8B2727C383F}"/>
+    <hyperlink ref="H72" r:id="rId72" xr:uid="{99C2B4AC-06EC-445C-AD10-96989F1C25E0}"/>
+    <hyperlink ref="H73" r:id="rId73" xr:uid="{86078F22-8AF1-44CD-BEAC-01233F855721}"/>
+    <hyperlink ref="H74" r:id="rId74" display="http://www.linkedin.com/in/suhana-shrestha" xr:uid="{53C26434-110F-4AF6-8CD6-9A93C8475C92}"/>
+    <hyperlink ref="H75" r:id="rId75" xr:uid="{6F73D0A1-C18C-438B-AC1D-94521C25804F}"/>
+    <hyperlink ref="H76" r:id="rId76" display="http://www.linkedin.com/in/tomisin-ojaokomo" xr:uid="{88EDD760-8E2F-43EC-9B0D-2FAD141AA86E}"/>
+    <hyperlink ref="H77" r:id="rId77" xr:uid="{F51A016D-E482-4ABD-94F9-394B4880D096}"/>
+    <hyperlink ref="H78" r:id="rId78" display="http://www.linkedin.com/in/utpal-prajapati-191a391a8" xr:uid="{B173318C-C519-4672-A834-1FF1FFF1A8E0}"/>
+    <hyperlink ref="H79" r:id="rId79" xr:uid="{6FE58E59-576D-40AD-821D-BAD2429E40BC}"/>
+    <hyperlink ref="D70" r:id="rId80" xr:uid="{807D2B8C-80E4-4EBE-A7F0-AC43AD49708C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId84"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId81"/>
   <tableParts count="1">
-    <tablePart r:id="rId85"/>
+    <tablePart r:id="rId82"/>
   </tableParts>
 </worksheet>
 </file>
@@ -4692,15 +4625,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DFB5B515010BFB41A71EECADA093B687" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="579b45423472ebbaf4eed9c56b664d89">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="11336436-e19c-451d-b666-d7c312f84b68" xmlns:ns3="b8d82043-2af1-4b83-b781-b5f1c44103c2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="95cf8f956f3c1dab4d6aa3fe57d77289" ns2:_="" ns3:_="">
     <xsd:import namespace="11336436-e19c-451d-b666-d7c312f84b68"/>
@@ -4913,32 +4837,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{965B0BEE-CA76-4190-A40E-2CA8E924EE1D}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="11336436-e19c-451d-b666-d7c312f84b68"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="11336436-e19c-451d-b666-d7c312f84b68"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="b8d82043-2af1-4b83-b781-b5f1c44103c2"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56BE6962-09DF-4C7A-9777-8A7F4643AC2E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB3CBDFA-9AAE-4389-9808-2150F2B25301}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4955,4 +4880,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56BE6962-09DF-4C7A-9777-8A7F4643AC2E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update: add new member photo, update TS output structure
</commit_message>
<xml_diff>
--- a/excel_input/Hackathon 2025 Organizing Team Member Profile Submission.xlsx
+++ b/excel_input/Hackathon 2025 Organizing Team Member Profile Submission.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28702"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28708"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pytest\excel_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{25C3FA0A-40DD-4D20-BCCA-F1C9A569603C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D9720360-18E6-4E5E-8A1A-A2DF68DE7BC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19020" yWindow="1464" windowWidth="21288" windowHeight="15012" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15420" yWindow="1932" windowWidth="21288" windowHeight="15012" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,8 +35,32 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="I112" authorId="0" shapeId="0" xr:uid="{63092EEC-E561-44FF-8C2E-3D61D7D2B058}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="宋体"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>回复者已更新此值。</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="619">
   <si>
     <t>Id</t>
   </si>
@@ -1813,6 +1837,124 @@
     <t>https://drive.google.com/file/d/1YbWDrn0URyo_Cttzwt7UJXAvJ_1ADkbU/view?usp=drive_link</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>Mehta Vidhi</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PMC</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=13yfYQuwjl0p1sHeaAD53Udc_WIu_FZ8G</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/harmanjot-singh-05807820b?utm_source=share&amp;utm_campaign=share_via&amp;utm_content=profile&amp;utm_medium=ios_app</t>
+  </si>
+  <si>
+    <t>Working in Registration Team</t>
+  </si>
+  <si>
+    <t>Haru Ai Okabe</t>
+  </si>
+  <si>
+    <t>Event and Media Production</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1kOulKtSTul33QovaultMkBFaSES_LupB</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/haru-ai/</t>
+  </si>
+  <si>
+    <t>Technical Lead</t>
+  </si>
+  <si>
+    <t>Talia Ghalayini</t>
+  </si>
+  <si>
+    <t>Computer Engineering Technology ECT</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1tlRIW1qw3tT9fN3NwsFQkMs4J0mByImr</t>
+  </si>
+  <si>
+    <t>www.linkedin.com/in/talia-ghalayini</t>
+  </si>
+  <si>
+    <t>communication manager</t>
+  </si>
+  <si>
+    <t>Bachelor's of Computer science (Honours)</t>
+  </si>
+  <si>
+    <t>Honours Bachelor of Technology – Software Development (BSD)</t>
+  </si>
+  <si>
+    <t>BSD</t>
+  </si>
+  <si>
+    <t>Alumni, CPA</t>
+  </si>
+  <si>
+    <t>Business Analytics</t>
+  </si>
+  <si>
+    <t>Web Development - Conestoga College</t>
+  </si>
+  <si>
+    <t>Computer Systems Technology</t>
+  </si>
+  <si>
+    <t>Bachelor of Computer Science (Honours)</t>
+  </si>
+  <si>
+    <t>project management IT (PMCC)</t>
+  </si>
+  <si>
+    <t>Project Management- Information Technology</t>
+  </si>
+  <si>
+    <t>York University- Digital marketing</t>
+  </si>
+  <si>
+    <t>Computer Systems Technician</t>
+  </si>
+  <si>
+    <t>EMP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bachelor's of Computer science </t>
+  </si>
+  <si>
+    <t>Diploma in Creative Advertising</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Digital And Content Marketing</t>
+  </si>
+  <si>
+    <t>Event and Media productions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Event And Media Production </t>
+  </si>
+  <si>
+    <t>Web Development</t>
+  </si>
+  <si>
+    <t>Project Management Information Technology</t>
+  </si>
+  <si>
+    <t>Accounting &amp; Finance (ACF</t>
+  </si>
+  <si>
+    <t>haokabe@myseneca.ca</t>
+  </si>
+  <si>
+    <t>tghalayini1@myseneca.ca</t>
+  </si>
 </sst>
 </file>
 
@@ -1821,7 +1963,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1884,6 +2026,22 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1893,7 +2051,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -2051,6 +2209,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF442F65"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFF8F9FA"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFF8F9FA"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFF8F9FA"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFF8F9FA"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFF8F9FA"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF442F65"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2058,7 +2244,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2116,6 +2302,50 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="176" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2198,8 +2428,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="OfficeForms.Table" displayName="OfficeForms.Table" ref="A1:K109" totalsRowShown="0">
-  <autoFilter ref="A1:K109" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="OfficeForms.Table" displayName="OfficeForms.Table" ref="A1:K112" totalsRowShown="0">
+  <autoFilter ref="A1:K112" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K66">
     <sortCondition ref="K1:K66"/>
   </sortState>
@@ -2599,11 +2829,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K109"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="G103" sqref="G103"/>
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="D110" sqref="D110:D112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -4676,7 +4906,7 @@
       </c>
       <c r="J64" s="2"/>
     </row>
-    <row r="65" spans="1:10" ht="115.2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" ht="115.2" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>23</v>
       </c>
@@ -4706,7 +4936,7 @@
       </c>
       <c r="J65" s="2"/>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>24</v>
       </c>
@@ -4736,7 +4966,7 @@
       </c>
       <c r="J66" s="2"/>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C67" s="11">
         <v>45719.799443171301</v>
       </c>
@@ -4759,8 +4989,11 @@
         <v>460</v>
       </c>
       <c r="J67" s="2"/>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K67" s="36" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C68" s="12">
         <v>45719.873041539351</v>
       </c>
@@ -4783,8 +5016,11 @@
         <v>430</v>
       </c>
       <c r="J68" s="2"/>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K68" s="34" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C69" s="11">
         <v>45719.88118034722</v>
       </c>
@@ -4807,8 +5043,11 @@
         <v>431</v>
       </c>
       <c r="J69" s="2"/>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K69" s="36" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C70" s="12">
         <v>45719.885935300925</v>
       </c>
@@ -4831,8 +5070,11 @@
         <v>463</v>
       </c>
       <c r="J70" s="2"/>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K70" s="34" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C71" s="11">
         <v>45719.886403645833</v>
       </c>
@@ -4855,8 +5097,11 @@
         <v>311</v>
       </c>
       <c r="J71" s="2"/>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K71" s="36" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C72" s="12">
         <v>45719.894827222219</v>
       </c>
@@ -4879,8 +5124,11 @@
         <v>432</v>
       </c>
       <c r="J72" s="2"/>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K72" s="34" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C73" s="11">
         <v>45719.954913437497</v>
       </c>
@@ -4905,8 +5153,11 @@
       <c r="J73" s="2" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K73" s="36" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C74" s="12">
         <v>45719.968188067127</v>
       </c>
@@ -4929,8 +5180,11 @@
         <v>464</v>
       </c>
       <c r="J74" s="2"/>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K74" s="34" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C75" s="11">
         <v>45719.979304247681</v>
       </c>
@@ -4953,8 +5207,11 @@
         <v>466</v>
       </c>
       <c r="J75" s="2"/>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K75" s="36" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C76" s="12">
         <v>45719.982414363425</v>
       </c>
@@ -4977,8 +5234,11 @@
         <v>434</v>
       </c>
       <c r="J76" s="2"/>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K76" s="34" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C77" s="11">
         <v>45719.999470196759</v>
       </c>
@@ -5001,8 +5261,11 @@
         <v>435</v>
       </c>
       <c r="J77" s="2"/>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K77" s="36" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C78" s="12">
         <v>45720.488428611112</v>
       </c>
@@ -5025,8 +5288,11 @@
         <v>469</v>
       </c>
       <c r="J78" s="2"/>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K78" s="34" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C79" s="11">
         <v>45720.654069224533</v>
       </c>
@@ -5049,8 +5315,11 @@
         <v>436</v>
       </c>
       <c r="J79" s="2"/>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K79" s="36" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C80" s="12">
         <v>45720.78224670139</v>
       </c>
@@ -5073,8 +5342,11 @@
         <v>437</v>
       </c>
       <c r="J80" s="2"/>
-    </row>
-    <row r="81" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K80" s="34" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="81" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C81" s="11">
         <v>45720.847401956024</v>
       </c>
@@ -5097,8 +5369,11 @@
         <v>472</v>
       </c>
       <c r="J81" s="2"/>
-    </row>
-    <row r="82" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K81" s="36" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="82" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C82" s="12">
         <v>45721.564685972218</v>
       </c>
@@ -5121,8 +5396,11 @@
         <v>476</v>
       </c>
       <c r="J82" s="2"/>
-    </row>
-    <row r="83" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K82" s="34" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="83" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C83" s="11">
         <v>45721.888644479171</v>
       </c>
@@ -5145,8 +5423,11 @@
         <v>438</v>
       </c>
       <c r="J83" s="2"/>
-    </row>
-    <row r="84" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K83" s="36" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="84" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C84" s="12">
         <v>45722.857292546294</v>
       </c>
@@ -5169,8 +5450,11 @@
         <v>480</v>
       </c>
       <c r="J84" s="2"/>
-    </row>
-    <row r="85" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K84" s="34" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="85" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C85" s="11">
         <v>45722.875584062502</v>
       </c>
@@ -5193,8 +5477,11 @@
         <v>476</v>
       </c>
       <c r="J85" s="2"/>
-    </row>
-    <row r="86" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K85" s="36" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="86" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C86" s="12">
         <v>45723.020868217594</v>
       </c>
@@ -5217,8 +5504,11 @@
         <v>484</v>
       </c>
       <c r="J86" s="2"/>
-    </row>
-    <row r="87" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K86" s="34" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="87" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C87" s="11">
         <v>45725.873511550926</v>
       </c>
@@ -5241,8 +5531,11 @@
         <v>487</v>
       </c>
       <c r="J87" s="2"/>
-    </row>
-    <row r="88" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K87" s="36" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="88" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C88" s="12">
         <v>45726.530941840276</v>
       </c>
@@ -5265,8 +5558,11 @@
         <v>489</v>
       </c>
       <c r="J88" s="2"/>
-    </row>
-    <row r="89" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K88" s="34" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="89" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C89" s="11">
         <v>45726.650853321757</v>
       </c>
@@ -5289,8 +5585,11 @@
         <v>491</v>
       </c>
       <c r="J89" s="2"/>
-    </row>
-    <row r="90" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K89" s="36" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="90" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C90" s="12">
         <v>45726.662231979164</v>
       </c>
@@ -5313,8 +5612,11 @@
         <v>495</v>
       </c>
       <c r="J90" s="2"/>
-    </row>
-    <row r="91" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K90" s="34" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="91" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C91" s="11">
         <v>45726.683793680553</v>
       </c>
@@ -5337,8 +5639,11 @@
         <v>497</v>
       </c>
       <c r="J91" s="2"/>
-    </row>
-    <row r="92" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K91" s="36" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="92" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C92" s="12">
         <v>45726.818197905093</v>
       </c>
@@ -5361,8 +5666,11 @@
         <v>501</v>
       </c>
       <c r="J92" s="2"/>
-    </row>
-    <row r="93" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K92" s="34" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="93" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C93" s="11">
         <v>45726.899962731477</v>
       </c>
@@ -5385,8 +5693,11 @@
         <v>524</v>
       </c>
       <c r="J93" s="2"/>
-    </row>
-    <row r="94" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K93" s="36" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="94" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C94" s="12">
         <v>45726.900201597222</v>
       </c>
@@ -5409,16 +5720,19 @@
         <v>526</v>
       </c>
       <c r="J94" s="2"/>
-    </row>
-    <row r="95" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K94" s="34" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="95" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C95" s="11">
         <v>45726.937757395834</v>
       </c>
       <c r="D95" s="23" t="s">
         <v>574</v>
       </c>
-      <c r="E95" s="14" t="s">
-        <v>511</v>
+      <c r="E95" s="25" t="s">
+        <v>580</v>
       </c>
       <c r="F95" s="14" t="s">
         <v>511</v>
@@ -5433,8 +5747,11 @@
         <v>529</v>
       </c>
       <c r="J95" s="2"/>
-    </row>
-    <row r="96" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K95" s="36" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="96" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C96" s="12">
         <v>45726.939952534725</v>
       </c>
@@ -5457,8 +5774,11 @@
         <v>532</v>
       </c>
       <c r="J96" s="2"/>
-    </row>
-    <row r="97" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K96" s="34" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C97" s="11">
         <v>45726.983095324074</v>
       </c>
@@ -5481,8 +5801,11 @@
         <v>534</v>
       </c>
       <c r="J97" s="2"/>
-    </row>
-    <row r="98" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K97" s="36" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C98" s="12">
         <v>45727.004515752313</v>
       </c>
@@ -5505,8 +5828,11 @@
         <v>537</v>
       </c>
       <c r="J98" s="2"/>
-    </row>
-    <row r="99" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K98" s="34" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C99" s="11">
         <v>45727.299762222217</v>
       </c>
@@ -5529,8 +5855,11 @@
         <v>540</v>
       </c>
       <c r="J99" s="2"/>
-    </row>
-    <row r="100" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K99" s="36" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C100" s="12">
         <v>45727.352533171295</v>
       </c>
@@ -5553,8 +5882,11 @@
         <v>542</v>
       </c>
       <c r="J100" s="2"/>
-    </row>
-    <row r="101" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K100" s="34" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C101" s="11">
         <v>45727.482564618054</v>
       </c>
@@ -5577,8 +5909,11 @@
         <v>544</v>
       </c>
       <c r="J101" s="2"/>
-    </row>
-    <row r="102" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K101" s="36" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C102" s="12">
         <v>45727.641773090276</v>
       </c>
@@ -5601,8 +5936,11 @@
         <v>547</v>
       </c>
       <c r="J102" s="2"/>
-    </row>
-    <row r="103" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K102" s="34" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C103" s="11">
         <v>45727.663368182868</v>
       </c>
@@ -5625,8 +5963,11 @@
         <v>177</v>
       </c>
       <c r="J103" s="2"/>
-    </row>
-    <row r="104" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K103" s="36" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C104" s="12">
         <v>45728.084605462966</v>
       </c>
@@ -5649,8 +5990,11 @@
         <v>551</v>
       </c>
       <c r="J104" s="2"/>
-    </row>
-    <row r="105" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K104" s="34" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C105" s="11">
         <v>45728.386568518516</v>
       </c>
@@ -5673,8 +6017,11 @@
         <v>553</v>
       </c>
       <c r="J105" s="2"/>
-    </row>
-    <row r="106" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K105" s="36" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C106" s="12">
         <v>45728.761242777779</v>
       </c>
@@ -5697,8 +6044,11 @@
         <v>556</v>
       </c>
       <c r="J106" s="2"/>
-    </row>
-    <row r="107" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K106" s="34" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C107" s="11">
         <v>45728.763991273147</v>
       </c>
@@ -5721,8 +6071,11 @@
         <v>559</v>
       </c>
       <c r="J107" s="2"/>
-    </row>
-    <row r="108" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K107" s="36" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C108" s="12">
         <v>45728.779622615737</v>
       </c>
@@ -5745,8 +6098,11 @@
         <v>562</v>
       </c>
       <c r="J108" s="2"/>
-    </row>
-    <row r="109" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K108" s="34" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C109" s="13">
         <v>45728.878916875001</v>
       </c>
@@ -5769,6 +6125,94 @@
         <v>564</v>
       </c>
       <c r="J109" s="2"/>
+      <c r="K109" s="36" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A110" s="28"/>
+      <c r="C110" s="26">
+        <v>45729.108823287039</v>
+      </c>
+      <c r="D110" s="40" t="s">
+        <v>302</v>
+      </c>
+      <c r="E110" s="34" t="s">
+        <v>303</v>
+      </c>
+      <c r="F110" s="34" t="s">
+        <v>303</v>
+      </c>
+      <c r="G110" s="35" t="s">
+        <v>582</v>
+      </c>
+      <c r="H110" s="35" t="s">
+        <v>583</v>
+      </c>
+      <c r="I110" s="34" t="s">
+        <v>584</v>
+      </c>
+      <c r="J110" s="29"/>
+      <c r="K110" s="34" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A111" s="28"/>
+      <c r="C111" s="27">
+        <v>45729.536587986113</v>
+      </c>
+      <c r="D111" s="41" t="s">
+        <v>617</v>
+      </c>
+      <c r="E111" s="36" t="s">
+        <v>585</v>
+      </c>
+      <c r="F111" s="36" t="s">
+        <v>585</v>
+      </c>
+      <c r="G111" s="37" t="s">
+        <v>587</v>
+      </c>
+      <c r="H111" s="37" t="s">
+        <v>588</v>
+      </c>
+      <c r="I111" s="36" t="s">
+        <v>589</v>
+      </c>
+      <c r="J111" s="29"/>
+      <c r="K111" s="36" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A112" s="30"/>
+      <c r="B112" s="31"/>
+      <c r="C112" s="32">
+        <v>45730.514499641205</v>
+      </c>
+      <c r="D112" s="42" t="s">
+        <v>618</v>
+      </c>
+      <c r="E112" s="38" t="s">
+        <v>590</v>
+      </c>
+      <c r="F112" s="38" t="s">
+        <v>590</v>
+      </c>
+      <c r="G112" s="39" t="s">
+        <v>592</v>
+      </c>
+      <c r="H112" s="39" t="s">
+        <v>593</v>
+      </c>
+      <c r="I112" s="38" t="s">
+        <v>594</v>
+      </c>
+      <c r="J112" s="33"/>
+      <c r="K112" s="38" t="s">
+        <v>591</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -5911,16 +6355,34 @@
     <hyperlink ref="H108" r:id="rId136" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
     <hyperlink ref="H109" r:id="rId137" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
     <hyperlink ref="H97" r:id="rId138" xr:uid="{FE4B5546-AF12-42FB-893D-AC0FAFA2FF07}"/>
+    <hyperlink ref="G110" r:id="rId139" xr:uid="{57051396-EDFB-4AAB-A1B4-6804F7A68A30}"/>
+    <hyperlink ref="H110" r:id="rId140" xr:uid="{AC13D95B-0612-4842-9D0E-CF79A4D02C67}"/>
+    <hyperlink ref="G111" r:id="rId141" xr:uid="{2FE2D665-BA15-44E8-8D45-B20284002192}"/>
+    <hyperlink ref="H111" r:id="rId142" xr:uid="{516E9B11-C6D7-46B1-AF77-3CC438A1CD8F}"/>
+    <hyperlink ref="G112" r:id="rId143" xr:uid="{845D3B0D-C280-452A-9164-E07C7A4AB1EF}"/>
+    <hyperlink ref="H112" r:id="rId144" xr:uid="{3B939D9F-06F7-40C1-8890-4997A28AA698}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId139"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId145"/>
+  <legacyDrawing r:id="rId146"/>
   <tableParts count="1">
-    <tablePart r:id="rId140"/>
+    <tablePart r:id="rId147"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="11336436-e19c-451d-b666-d7c312f84b68">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b8d82043-2af1-4b83-b781-b5f1c44103c2" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DFB5B515010BFB41A71EECADA093B687" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="579b45423472ebbaf4eed9c56b664d89">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="11336436-e19c-451d-b666-d7c312f84b68" xmlns:ns3="b8d82043-2af1-4b83-b781-b5f1c44103c2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="95cf8f956f3c1dab4d6aa3fe57d77289" ns2:_="" ns3:_="">
     <xsd:import namespace="11336436-e19c-451d-b666-d7c312f84b68"/>
@@ -6133,7 +6595,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -6142,18 +6604,24 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="11336436-e19c-451d-b666-d7c312f84b68">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b8d82043-2af1-4b83-b781-b5f1c44103c2" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{965B0BEE-CA76-4190-A40E-2CA8E924EE1D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="11336436-e19c-451d-b666-d7c312f84b68"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="b8d82043-2af1-4b83-b781-b5f1c44103c2"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB3CBDFA-9AAE-4389-9808-2150F2B25301}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6172,27 +6640,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56BE6962-09DF-4C7A-9777-8A7F4643AC2E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{965B0BEE-CA76-4190-A40E-2CA8E924EE1D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="11336436-e19c-451d-b666-d7c312f84b68"/>
-    <ds:schemaRef ds:uri="b8d82043-2af1-4b83-b781-b5f1c44103c2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>